<commit_message>
One click introduction a příprava na oboustrannou komunikaci
</commit_message>
<xml_diff>
--- a/timeline/3M Project Timeline.xlsx
+++ b/timeline/3M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0BB2ECC-A4C6-4EDC-8153-C1BA2DB5DB5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D89645-B370-4C15-A4C1-7D03966E6724}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -524,6 +524,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -533,15 +569,9 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,36 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -833,7 +833,7 @@
   <dimension ref="B1:AF28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15:T15"/>
+      <selection activeCell="AE15" sqref="AE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -847,91 +847,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="44" t="s">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35"/>
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="46">
+      <c r="C2" s="37">
         <v>43199</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="45" t="s">
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="45"/>
-      <c r="L4" s="45"/>
-      <c r="M4" s="45"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="45"/>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="47" t="s">
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="47"/>
-      <c r="S4" s="47"/>
-      <c r="T4" s="47"/>
-      <c r="U4" s="47"/>
-      <c r="V4" s="47"/>
-      <c r="W4" s="47"/>
-      <c r="X4" s="45" t="s">
+      <c r="R4" s="38"/>
+      <c r="S4" s="38"/>
+      <c r="T4" s="38"/>
+      <c r="U4" s="38"/>
+      <c r="V4" s="38"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="45"/>
-      <c r="AA4" s="45"/>
-      <c r="AB4" s="45"/>
-      <c r="AC4" s="45"/>
-      <c r="AD4" s="45"/>
-      <c r="AE4" s="42" t="s">
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="33" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1052,7 +1052,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="42"/>
+      <c r="AE5" s="33"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1171,7 +1171,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="42"/>
+      <c r="AE6" s="33"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1289,24 +1289,24 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43226</v>
       </c>
-      <c r="AE7" s="43"/>
+      <c r="AE7" s="34"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
       <c r="M8" s="24"/>
       <c r="N8" s="25"/>
       <c r="O8" s="24"/>
@@ -1325,7 +1325,7 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="48" t="s">
+      <c r="AE8" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1333,23 +1333,23 @@
       <c r="B9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="32"/>
+      <c r="Q9" s="32"/>
       <c r="R9" s="6"/>
       <c r="S9" s="5"/>
       <c r="T9" s="6"/>
@@ -1363,7 +1363,7 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="5"/>
       <c r="AD9" s="6"/>
-      <c r="AE9" s="48" t="s">
+      <c r="AE9" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1371,18 +1371,18 @@
       <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
       <c r="M10" s="26"/>
       <c r="N10" s="27"/>
       <c r="O10" s="26"/>
@@ -1401,7 +1401,7 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="48" t="s">
+      <c r="AE10" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1439,7 +1439,7 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="48" t="s">
+      <c r="AE11" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1447,18 +1447,18 @@
       <c r="B12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="41"/>
       <c r="M12" s="24"/>
       <c r="N12" s="25"/>
       <c r="O12" s="24"/>
@@ -1477,7 +1477,7 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="48" t="s">
+      <c r="AE12" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1490,16 +1490,16 @@
       <c r="E13" s="28"/>
       <c r="F13" s="29"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="33" t="s">
+      <c r="H13" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="33"/>
-      <c r="L13" s="33"/>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
@@ -1515,7 +1515,7 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="6"/>
-      <c r="AE13" s="48" t="s">
+      <c r="AE13" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1553,7 +1553,7 @@
       <c r="AB14" s="6"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="6"/>
-      <c r="AE14" s="48" t="s">
+      <c r="AE14" s="30" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1608,15 +1608,15 @@
       <c r="K16" s="26"/>
       <c r="L16" s="27"/>
       <c r="M16" s="26"/>
-      <c r="N16" s="33" t="s">
+      <c r="N16" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="33"/>
-      <c r="P16" s="33"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="33"/>
-      <c r="T16" s="33"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="32"/>
+      <c r="R16" s="32"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
       <c r="W16" s="5"/>
@@ -1627,7 +1627,9 @@
       <c r="AB16" s="6"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="6"/>
-      <c r="AE16" s="20"/>
+      <c r="AE16" s="30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="17" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
@@ -1679,15 +1681,15 @@
       <c r="J18" s="6"/>
       <c r="K18" s="5"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
       <c r="T18" s="6"/>
       <c r="U18" s="5"/>
       <c r="V18" s="6"/>
@@ -1724,17 +1726,17 @@
       <c r="S19" s="5"/>
       <c r="T19" s="6"/>
       <c r="U19" s="5"/>
-      <c r="V19" s="36" t="s">
+      <c r="V19" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="W19" s="37"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="37"/>
-      <c r="Z19" s="37"/>
-      <c r="AA19" s="37"/>
-      <c r="AB19" s="37"/>
-      <c r="AC19" s="37"/>
-      <c r="AD19" s="38"/>
+      <c r="W19" s="47"/>
+      <c r="X19" s="47"/>
+      <c r="Y19" s="47"/>
+      <c r="Z19" s="47"/>
+      <c r="AA19" s="47"/>
+      <c r="AB19" s="47"/>
+      <c r="AC19" s="47"/>
+      <c r="AD19" s="48"/>
       <c r="AE19" s="20"/>
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1757,13 +1759,13 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="35" t="s">
+      <c r="S20" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="T20" s="35"/>
-      <c r="U20" s="35"/>
-      <c r="V20" s="35"/>
-      <c r="W20" s="35"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="5"/>
       <c r="Z20" s="6"/>
@@ -1797,16 +1799,16 @@
       <c r="T21" s="6"/>
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
-      <c r="W21" s="30" t="s">
+      <c r="W21" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="X21" s="31"/>
-      <c r="Y21" s="31"/>
-      <c r="Z21" s="31"/>
-      <c r="AA21" s="31"/>
-      <c r="AB21" s="31"/>
-      <c r="AC21" s="31"/>
-      <c r="AD21" s="32"/>
+      <c r="X21" s="43"/>
+      <c r="Y21" s="43"/>
+      <c r="Z21" s="43"/>
+      <c r="AA21" s="43"/>
+      <c r="AB21" s="43"/>
+      <c r="AC21" s="43"/>
+      <c r="AD21" s="44"/>
       <c r="AE21" s="20"/>
     </row>
     <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1830,20 +1832,22 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="6"/>
       <c r="S22" s="5"/>
-      <c r="T22" s="33" t="s">
+      <c r="T22" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="U22" s="33"/>
-      <c r="V22" s="33"/>
-      <c r="W22" s="33"/>
-      <c r="X22" s="33"/>
-      <c r="Y22" s="33"/>
-      <c r="Z22" s="33"/>
+      <c r="U22" s="32"/>
+      <c r="V22" s="32"/>
+      <c r="W22" s="32"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="5"/>
       <c r="AD22" s="6"/>
-      <c r="AE22" s="20"/>
+      <c r="AE22" s="30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="23" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
@@ -1870,15 +1874,15 @@
       <c r="U23" s="7"/>
       <c r="V23" s="8"/>
       <c r="W23" s="7"/>
-      <c r="X23" s="34" t="s">
+      <c r="X23" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="34"/>
-      <c r="Z23" s="34"/>
-      <c r="AA23" s="34"/>
-      <c r="AB23" s="34"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="34"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="45"/>
+      <c r="AA23" s="45"/>
+      <c r="AB23" s="45"/>
+      <c r="AC23" s="45"/>
+      <c r="AD23" s="45"/>
       <c r="AE23" s="20"/>
     </row>
     <row r="24" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2043,6 +2047,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="W21:AD21"/>
+    <mergeCell ref="T22:Z22"/>
+    <mergeCell ref="X23:AD23"/>
+    <mergeCell ref="M18:S18"/>
+    <mergeCell ref="V19:AD19"/>
+    <mergeCell ref="S20:W20"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="K15:T15"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="N16:T16"/>
+    <mergeCell ref="Q17:X17"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="H13:O13"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:Q9"/>
     <mergeCell ref="AE4:AE7"/>
@@ -2052,20 +2070,6 @@
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="K15:T15"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="N16:T16"/>
-    <mergeCell ref="Q17:X17"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="H13:O13"/>
-    <mergeCell ref="W21:AD21"/>
-    <mergeCell ref="T22:Z22"/>
-    <mergeCell ref="X23:AD23"/>
-    <mergeCell ref="M18:S18"/>
-    <mergeCell ref="V19:AD19"/>
-    <mergeCell ref="S20:W20"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Timelajna pro poslední měsíc a vydání
</commit_message>
<xml_diff>
--- a/timeline/3M Project Timeline.xlsx
+++ b/timeline/3M Project Timeline.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\ZPR\Backupper\timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7C68FE-0471-47BC-9ECA-9E4467A17542}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Timeline" sheetId="1" r:id="rId1"/>
@@ -17,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Timeline'!$4:$7</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -125,7 +126,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="mmm"/>
@@ -526,12 +527,42 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -550,49 +581,19 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="11">
-    <cellStyle name="Date" xfId="6"/>
-    <cellStyle name="Day of week" xfId="8"/>
-    <cellStyle name="Month" xfId="9"/>
-    <cellStyle name="Nadpis 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Nadpis 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Nadpis 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Nadpis 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Název" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Status" xfId="10"/>
-    <cellStyle name="Weekday" xfId="7"/>
+    <cellStyle name="Date" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Day of week" xfId="8" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Month" xfId="9" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Status" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Weekday" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -824,15 +825,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="9"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
   <dimension ref="B1:AF28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE20" sqref="AE20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -846,91 +847,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35"/>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35"/>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
+      <c r="J1" s="45"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
+      <c r="M1" s="45"/>
+      <c r="N1" s="45"/>
+      <c r="O1" s="45"/>
+      <c r="P1" s="45"/>
+      <c r="Q1" s="45"/>
+      <c r="R1" s="45"/>
+      <c r="S1" s="45"/>
+      <c r="T1" s="45"/>
+      <c r="U1" s="45"/>
+      <c r="V1" s="45"/>
+      <c r="W1" s="45"/>
+      <c r="X1" s="45"/>
+      <c r="Y1" s="45"/>
+      <c r="Z1" s="45"/>
+      <c r="AA1" s="45"/>
+      <c r="AB1" s="45"/>
+      <c r="AC1" s="45"/>
+      <c r="AD1" s="45"/>
+      <c r="AE1" s="45"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="47">
         <v>43199</v>
       </c>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="38" t="s">
+      <c r="C4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="36" t="s">
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="38" t="s">
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="38"/>
-      <c r="S4" s="38"/>
-      <c r="T4" s="38"/>
-      <c r="U4" s="38"/>
-      <c r="V4" s="38"/>
-      <c r="W4" s="38"/>
-      <c r="X4" s="36" t="s">
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
-      <c r="AE4" s="33" t="s">
+      <c r="Y4" s="46"/>
+      <c r="Z4" s="46"/>
+      <c r="AA4" s="46"/>
+      <c r="AB4" s="46"/>
+      <c r="AC4" s="46"/>
+      <c r="AD4" s="46"/>
+      <c r="AE4" s="43" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1051,7 +1052,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="33"/>
+      <c r="AE5" s="43"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1170,7 +1171,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="33"/>
+      <c r="AE6" s="43"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1288,24 +1289,24 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43226</v>
       </c>
-      <c r="AE7" s="34"/>
+      <c r="AE7" s="44"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="31"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="42"/>
       <c r="M8" s="24"/>
       <c r="N8" s="25"/>
       <c r="O8" s="24"/>
@@ -1332,23 +1333,23 @@
       <c r="B9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
-      <c r="J9" s="32"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="32"/>
-      <c r="M9" s="32"/>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="P9" s="32"/>
-      <c r="Q9" s="32"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="34"/>
+      <c r="G9" s="34"/>
+      <c r="H9" s="34"/>
+      <c r="I9" s="34"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
       <c r="R9" s="6"/>
       <c r="S9" s="5"/>
       <c r="T9" s="6"/>
@@ -1370,18 +1371,18 @@
       <c r="B10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
       <c r="M10" s="26"/>
       <c r="N10" s="27"/>
       <c r="O10" s="26"/>
@@ -1408,18 +1409,18 @@
       <c r="B11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
       <c r="M11" s="5"/>
       <c r="N11" s="6"/>
       <c r="O11" s="5"/>
@@ -1446,18 +1447,18 @@
       <c r="B12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="41"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
+      <c r="H12" s="36"/>
+      <c r="I12" s="36"/>
+      <c r="J12" s="36"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="36"/>
       <c r="M12" s="24"/>
       <c r="N12" s="25"/>
       <c r="O12" s="24"/>
@@ -1489,16 +1490,16 @@
       <c r="E13" s="28"/>
       <c r="F13" s="29"/>
       <c r="G13" s="28"/>
-      <c r="H13" s="32" t="s">
+      <c r="H13" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
@@ -1522,16 +1523,16 @@
       <c r="B14" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="28"/>
       <c r="L14" s="29"/>
       <c r="M14" s="28"/>
@@ -1568,18 +1569,18 @@
       <c r="H15" s="27"/>
       <c r="I15" s="26"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="40" t="s">
+      <c r="K15" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="L15" s="40"/>
-      <c r="M15" s="40"/>
-      <c r="N15" s="40"/>
-      <c r="O15" s="40"/>
-      <c r="P15" s="40"/>
-      <c r="Q15" s="40"/>
-      <c r="R15" s="40"/>
-      <c r="S15" s="40"/>
-      <c r="T15" s="40"/>
+      <c r="L15" s="41"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="41"/>
+      <c r="P15" s="41"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
       <c r="U15" s="5"/>
       <c r="V15" s="6"/>
       <c r="W15" s="5"/>
@@ -1590,7 +1591,9 @@
       <c r="AB15" s="6"/>
       <c r="AC15" s="5"/>
       <c r="AD15" s="6"/>
-      <c r="AE15" s="20"/>
+      <c r="AE15" s="30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
@@ -1607,15 +1610,15 @@
       <c r="K16" s="26"/>
       <c r="L16" s="27"/>
       <c r="M16" s="26"/>
-      <c r="N16" s="32" t="s">
+      <c r="N16" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="32"/>
-      <c r="P16" s="32"/>
-      <c r="Q16" s="32"/>
-      <c r="R16" s="32"/>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
+      <c r="O16" s="34"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="34"/>
+      <c r="R16" s="34"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
       <c r="W16" s="5"/>
@@ -1648,23 +1651,25 @@
       <c r="N17" s="6"/>
       <c r="O17" s="5"/>
       <c r="P17" s="6"/>
-      <c r="Q17" s="40" t="s">
+      <c r="Q17" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
-      <c r="X17" s="40"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
       <c r="Y17" s="5"/>
       <c r="Z17" s="6"/>
       <c r="AA17" s="5"/>
       <c r="AB17" s="6"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
-      <c r="AE17" s="20"/>
+      <c r="AE17" s="30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
@@ -1680,15 +1685,15 @@
       <c r="J18" s="6"/>
       <c r="K18" s="5"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="41" t="s">
+      <c r="M18" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="N18" s="41"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="41"/>
-      <c r="Q18" s="41"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="41"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="36"/>
+      <c r="P18" s="36"/>
+      <c r="Q18" s="36"/>
+      <c r="R18" s="36"/>
+      <c r="S18" s="36"/>
       <c r="T18" s="6"/>
       <c r="U18" s="5"/>
       <c r="V18" s="6"/>
@@ -1727,18 +1732,20 @@
       <c r="S19" s="5"/>
       <c r="T19" s="6"/>
       <c r="U19" s="5"/>
-      <c r="V19" s="46" t="s">
+      <c r="V19" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="W19" s="47"/>
-      <c r="X19" s="47"/>
-      <c r="Y19" s="47"/>
-      <c r="Z19" s="47"/>
-      <c r="AA19" s="47"/>
-      <c r="AB19" s="47"/>
-      <c r="AC19" s="47"/>
-      <c r="AD19" s="48"/>
-      <c r="AE19" s="20"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="Y19" s="38"/>
+      <c r="Z19" s="38"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="38"/>
+      <c r="AC19" s="38"/>
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="30" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
@@ -1760,13 +1767,13 @@
       <c r="P20" s="6"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="41" t="s">
+      <c r="S20" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
+      <c r="T20" s="36"/>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="5"/>
       <c r="Z20" s="6"/>
@@ -1802,16 +1809,16 @@
       <c r="T21" s="6"/>
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
-      <c r="W21" s="42" t="s">
+      <c r="W21" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="X21" s="43"/>
-      <c r="Y21" s="43"/>
-      <c r="Z21" s="43"/>
-      <c r="AA21" s="43"/>
-      <c r="AB21" s="43"/>
-      <c r="AC21" s="43"/>
-      <c r="AD21" s="44"/>
+      <c r="X21" s="32"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+      <c r="AA21" s="32"/>
+      <c r="AB21" s="32"/>
+      <c r="AC21" s="32"/>
+      <c r="AD21" s="33"/>
       <c r="AE21" s="30" t="s">
         <v>29</v>
       </c>
@@ -1837,15 +1844,15 @@
       <c r="Q22" s="5"/>
       <c r="R22" s="6"/>
       <c r="S22" s="5"/>
-      <c r="T22" s="32" t="s">
+      <c r="T22" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="U22" s="32"/>
-      <c r="V22" s="32"/>
-      <c r="W22" s="32"/>
-      <c r="X22" s="32"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="34"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
       <c r="AA22" s="5"/>
       <c r="AB22" s="6"/>
       <c r="AC22" s="5"/>
@@ -1879,15 +1886,15 @@
       <c r="U23" s="7"/>
       <c r="V23" s="8"/>
       <c r="W23" s="7"/>
-      <c r="X23" s="45" t="s">
+      <c r="X23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="45"/>
-      <c r="AA23" s="45"/>
-      <c r="AB23" s="45"/>
-      <c r="AC23" s="45"/>
-      <c r="AD23" s="45"/>
+      <c r="Y23" s="35"/>
+      <c r="Z23" s="35"/>
+      <c r="AA23" s="35"/>
+      <c r="AB23" s="35"/>
+      <c r="AC23" s="35"/>
+      <c r="AD23" s="35"/>
       <c r="AE23" s="30" t="s">
         <v>29</v>
       </c>
@@ -2054,20 +2061,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="W21:AD21"/>
-    <mergeCell ref="T22:Z22"/>
-    <mergeCell ref="X23:AD23"/>
-    <mergeCell ref="M18:S18"/>
-    <mergeCell ref="V19:AD19"/>
-    <mergeCell ref="S20:W20"/>
-    <mergeCell ref="C14:J14"/>
-    <mergeCell ref="K15:T15"/>
-    <mergeCell ref="C10:L10"/>
-    <mergeCell ref="N16:T16"/>
-    <mergeCell ref="Q17:X17"/>
-    <mergeCell ref="C11:L11"/>
-    <mergeCell ref="C12:L12"/>
-    <mergeCell ref="H13:O13"/>
     <mergeCell ref="C8:L8"/>
     <mergeCell ref="C9:Q9"/>
     <mergeCell ref="AE4:AE7"/>
@@ -2077,22 +2070,36 @@
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="C14:J14"/>
+    <mergeCell ref="K15:T15"/>
+    <mergeCell ref="C10:L10"/>
+    <mergeCell ref="N16:T16"/>
+    <mergeCell ref="Q17:X17"/>
+    <mergeCell ref="C11:L11"/>
+    <mergeCell ref="C12:L12"/>
+    <mergeCell ref="H13:O13"/>
+    <mergeCell ref="W21:AD21"/>
+    <mergeCell ref="T22:Z22"/>
+    <mergeCell ref="X23:AD23"/>
+    <mergeCell ref="M18:S18"/>
+    <mergeCell ref="V19:AD19"/>
+    <mergeCell ref="S20:W20"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>C$7=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="9">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter Start Date in cell C2 and other details starting in cell B4" sqref="A1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="B2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell" sqref="C2:E2"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell" sqref="B1:AE1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Days of the week are automatically updated in this row. Enter assigned to person's name in cells below and their tasks in the row at right of their name" sqref="B7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Update task status in cells below for each task assigned to a person in column B" sqref="AE4:AE7"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Week number is in cell blocks C to I, J to P, Q to W and X to AD in this row" sqref="B4"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Month is automatically updated in this row" sqref="B5"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Weekdays are automatically updated in this row" sqref="B6"/>
+  <dataValidations count="9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter Start Date in cell C2 and other details starting in cell B4" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell" sqref="C2:E2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of this worksheet is in this cell" sqref="B1:AE1" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Days of the week are automatically updated in this row. Enter assigned to person's name in cells below and their tasks in the row at right of their name" sqref="B7" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Update task status in cells below for each task assigned to a person in column B" sqref="AE4:AE7" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Week number is in cell blocks C to I, J to P, Q to W and X to AD in this row" sqref="B4" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Month is automatically updated in this row" sqref="B5" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Weekdays are automatically updated in this row" sqref="B6" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>